<commit_message>
Changes at end of sprint 2
</commit_message>
<xml_diff>
--- a/RPS FCPR - Technical and Functional Knowledge Matrix.xlsx
+++ b/RPS FCPR - Technical and Functional Knowledge Matrix.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="97">
   <si>
     <t>Topics</t>
   </si>
@@ -206,12 +206,6 @@
     <t>Deployment</t>
   </si>
   <si>
-    <t>June'15</t>
-  </si>
-  <si>
-    <t>Jun'15</t>
-  </si>
-  <si>
     <t>Abin Zachariah</t>
   </si>
   <si>
@@ -282,6 +276,45 @@
   </si>
   <si>
     <t>JIRA</t>
+  </si>
+  <si>
+    <t>Increase Domain knowledge</t>
+  </si>
+  <si>
+    <t>Sandarbh Sharma</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Increase Technical Knowledge</t>
+  </si>
+  <si>
+    <t>Team is learning fast, and have gained confidence in tchnology now</t>
+  </si>
+  <si>
+    <t>Constant interaction with business is bringing about change</t>
+  </si>
+  <si>
+    <t>N A</t>
+  </si>
+  <si>
+    <t>Training for Scala</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Trainier for scala was recruited to train the team and ensure they come up to speed</t>
+  </si>
+  <si>
+    <t>15/09/2015</t>
+  </si>
+  <si>
+    <t>August'15</t>
+  </si>
+  <si>
+    <t>September'15</t>
   </si>
 </sst>
 </file>
@@ -422,7 +455,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -838,12 +871,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -956,12 +998,6 @@
     <xf numFmtId="166" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -978,6 +1014,49 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -993,19 +1072,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1031,31 +1098,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1067,12 +1117,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1087,17 +1131,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1105,17 +1143,418 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="84">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1344,6 +1783,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:view3D>
       <c:depthPercent val="100"/>
@@ -1363,7 +1803,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>June'15</c:v>
+                  <c:v>August'15</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1416,13 +1856,75 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Functional Analysis'!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>September'15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Functional Analysis'!$B$7:$F$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Not Aware</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Beginner</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Intermediate</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Advanced</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Proficient</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Functional Analysis'!$B$9:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.2500000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.7499999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.51249999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="162840960"/>
-        <c:axId val="162842496"/>
+        <c:axId val="68942848"/>
+        <c:axId val="71108096"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="162840960"/>
+        <c:axId val="68942848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1447,14 +1949,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162842496"/>
+        <c:crossAx val="71108096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="162842496"/>
+        <c:axId val="71108096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1520,7 +2022,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162840960"/>
+        <c:crossAx val="68942848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1576,7 +2078,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1609,6 +2111,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:view3D>
       <c:depthPercent val="100"/>
@@ -1628,7 +2131,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Jun'15</c:v>
+                  <c:v>August'15</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1681,13 +2184,75 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Technical Analysis'!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>September'15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Technical Analysis'!$B$7:$F$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Not Aware</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Beginner</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Intermediate</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Advanced</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Proficient</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Technical Analysis'!$B$9:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.1081081081081086E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.54054054054054057</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3783783783783784</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:shape val="cylinder"/>
-        <c:axId val="162648448"/>
-        <c:axId val="162649984"/>
+        <c:axId val="72237056"/>
+        <c:axId val="72238592"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="162648448"/>
+        <c:axId val="72237056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1712,14 +2277,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162649984"/>
+        <c:crossAx val="72238592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="162649984"/>
+        <c:axId val="72238592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1785,7 +2350,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162648448"/>
+        <c:crossAx val="72237056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1841,7 +2406,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2716,12 +3281,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
-      <c r="A1" s="76"/>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="78"/>
+      <c r="A1" s="62"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="64"/>
       <c r="G1" s="30"/>
       <c r="H1" s="30"/>
       <c r="I1" s="30"/>
@@ -2748,12 +3313,12 @@
       <c r="AD1" s="30"/>
     </row>
     <row r="2" spans="1:30">
-      <c r="A2" s="79"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="81"/>
+      <c r="A2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="67"/>
       <c r="G2" s="30"/>
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
@@ -2780,12 +3345,12 @@
       <c r="AD2" s="30"/>
     </row>
     <row r="3" spans="1:30">
-      <c r="A3" s="79"/>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="81"/>
+      <c r="A3" s="65"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="67"/>
       <c r="G3" s="30"/>
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
@@ -2812,12 +3377,12 @@
       <c r="AD3" s="30"/>
     </row>
     <row r="4" spans="1:30">
-      <c r="A4" s="79"/>
-      <c r="B4" s="80"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="81"/>
+      <c r="A4" s="65"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="67"/>
       <c r="G4" s="30"/>
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
@@ -2844,12 +3409,12 @@
       <c r="AD4" s="30"/>
     </row>
     <row r="5" spans="1:30" ht="38.25" customHeight="1" thickBot="1">
-      <c r="A5" s="79"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="81"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="67"/>
       <c r="G5" s="30"/>
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
@@ -2876,18 +3441,18 @@
       <c r="AD5" s="30"/>
     </row>
     <row r="6" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="83"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="75" t="s">
+      <c r="D6" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="64"/>
-      <c r="F6" s="65"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="61"/>
       <c r="G6" s="30"/>
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
@@ -2914,18 +3479,18 @@
       <c r="AD6" s="30"/>
     </row>
     <row r="7" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="62"/>
+      <c r="B7" s="58"/>
       <c r="C7" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="84">
+      <c r="D7" s="70">
         <v>1</v>
       </c>
-      <c r="E7" s="85"/>
-      <c r="F7" s="86"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="72"/>
       <c r="G7" s="30"/>
       <c r="H7" s="30"/>
       <c r="I7" s="30"/>
@@ -2952,18 +3517,18 @@
       <c r="AD7" s="30"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="62"/>
+      <c r="B8" s="58"/>
       <c r="C8" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="75" t="s">
+      <c r="D8" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="64"/>
-      <c r="F8" s="65"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="61"/>
       <c r="G8" s="30"/>
       <c r="H8" s="30"/>
       <c r="I8" s="30"/>
@@ -2990,18 +3555,18 @@
       <c r="AD8" s="30"/>
     </row>
     <row r="9" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="62"/>
+      <c r="B9" s="58"/>
       <c r="C9" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="63" t="s">
+      <c r="D9" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="64"/>
-      <c r="F9" s="65"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="61"/>
       <c r="G9" s="30"/>
       <c r="H9" s="30"/>
       <c r="I9" s="30"/>
@@ -3028,18 +3593,18 @@
       <c r="AD9" s="30"/>
     </row>
     <row r="10" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A10" s="61" t="s">
+      <c r="A10" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="62"/>
+      <c r="B10" s="58"/>
       <c r="C10" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="66">
+      <c r="D10" s="79">
         <v>41954</v>
       </c>
-      <c r="E10" s="67"/>
-      <c r="F10" s="68"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="81"/>
       <c r="G10" s="30"/>
       <c r="H10" s="30"/>
       <c r="I10" s="30"/>
@@ -3098,13 +3663,13 @@
       <c r="AD11" s="30"/>
     </row>
     <row r="12" spans="1:30">
-      <c r="A12" s="69" t="s">
+      <c r="A12" s="82" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="70"/>
+      <c r="B12" s="83"/>
       <c r="C12" s="37"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
       <c r="F12" s="38"/>
       <c r="G12" s="30"/>
       <c r="H12" s="30"/>
@@ -3132,11 +3697,11 @@
       <c r="AD12" s="30"/>
     </row>
     <row r="13" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A13" s="71"/>
-      <c r="B13" s="72"/>
+      <c r="A13" s="84"/>
+      <c r="B13" s="85"/>
       <c r="C13" s="39"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="87"/>
       <c r="F13" s="40"/>
       <c r="G13" s="30"/>
       <c r="H13" s="30"/>
@@ -3167,10 +3732,10 @@
       <c r="A14" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="56"/>
+      <c r="C14" s="73"/>
       <c r="D14" s="42" t="s">
         <v>42</v>
       </c>
@@ -3206,13 +3771,13 @@
       <c r="AD14" s="30"/>
     </row>
     <row r="15" spans="1:30" ht="31.5" customHeight="1" thickBot="1">
-      <c r="A15" s="50">
+      <c r="A15" s="48">
         <v>1</v>
       </c>
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="58"/>
+      <c r="C15" s="75"/>
       <c r="D15" s="47" t="s">
         <v>55</v>
       </c>
@@ -3248,13 +3813,13 @@
       <c r="AD15" s="30"/>
     </row>
     <row r="16" spans="1:30" ht="31.5" customHeight="1">
-      <c r="A16" s="50">
+      <c r="A16" s="48">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="76" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="60"/>
+      <c r="C16" s="77"/>
       <c r="D16" s="47"/>
       <c r="E16" s="45">
         <v>41682</v>
@@ -7217,13 +7782,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="A1:F5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:F7"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
@@ -7234,6 +7792,13 @@
     <mergeCell ref="A12:B13"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="A1:F5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7245,10 +7810,10 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J3" sqref="J3:L3"/>
+      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7269,67 +7834,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75">
-      <c r="B1" s="88" t="s">
+      <c r="B1" s="106" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="108"/>
       <c r="M1" s="24"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="93" t="s">
+      <c r="C2" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="95" t="s">
+      <c r="D2" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="91" t="s">
+      <c r="E2" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="55"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="53"/>
       <c r="M2" s="24"/>
     </row>
     <row r="3" spans="1:13" ht="31.5" customHeight="1">
-      <c r="B3" s="94"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="96"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="98"/>
       <c r="E3" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="H3" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="I3" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="J3" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="K3" s="24" t="s">
         <v>66</v>
-      </c>
-      <c r="J3" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="K3" s="24" t="s">
-        <v>68</v>
       </c>
       <c r="L3" s="24" t="s">
         <v>58</v>
@@ -7339,11 +7904,11 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="103" t="s">
-        <v>69</v>
+      <c r="C4" s="54" t="s">
+        <v>67</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>9</v>
@@ -7375,12 +7940,12 @@
       <c r="M4" s="7"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="B5" s="87"/>
-      <c r="C5" s="103" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>5</v>
+      <c r="B5" s="91"/>
+      <c r="C5" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>9</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>9</v>
@@ -7409,12 +7974,12 @@
       <c r="M5" s="7"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="B6" s="87"/>
-      <c r="C6" s="103" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>5</v>
+      <c r="B6" s="91"/>
+      <c r="C6" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>9</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>9</v>
@@ -7443,12 +8008,12 @@
       <c r="M6" s="7"/>
     </row>
     <row r="7" spans="1:13" ht="14.25" customHeight="1">
-      <c r="B7" s="87"/>
-      <c r="C7" s="103" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>5</v>
+      <c r="B7" s="91"/>
+      <c r="C7" s="54" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>9</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>9</v>
@@ -7465,8 +8030,8 @@
       <c r="I7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="4" t="s">
-        <v>6</v>
+      <c r="J7" s="26" t="s">
+        <v>5</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>5</v>
@@ -7477,12 +8042,12 @@
       <c r="M7" s="7"/>
     </row>
     <row r="8" spans="1:13" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="B8" s="87"/>
-      <c r="C8" s="104" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>5</v>
+      <c r="B8" s="91"/>
+      <c r="C8" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>9</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>9</v>
@@ -7493,8 +8058,8 @@
       <c r="G8" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="7" t="s">
-        <v>6</v>
+      <c r="H8" s="26" t="s">
+        <v>5</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>5</v>
@@ -7502,8 +8067,8 @@
       <c r="J8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="7" t="s">
-        <v>6</v>
+      <c r="K8" s="26" t="s">
+        <v>5</v>
       </c>
       <c r="L8" s="14" t="s">
         <v>9</v>
@@ -7512,12 +8077,12 @@
     </row>
     <row r="9" spans="1:13" s="27" customFormat="1">
       <c r="A9"/>
-      <c r="B9" s="87"/>
-      <c r="C9" s="104" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>5</v>
+      <c r="B9" s="91"/>
+      <c r="C9" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>9</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>9</v>
@@ -7546,14 +8111,14 @@
       <c r="M9" s="7"/>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1">
-      <c r="B10" s="87" t="s">
+      <c r="B10" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="103" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>5</v>
+      <c r="C10" s="54" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>9</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>9</v>
@@ -7582,12 +8147,12 @@
       <c r="M10" s="7"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="B11" s="87"/>
-      <c r="C11" s="104" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>5</v>
+      <c r="B11" s="91"/>
+      <c r="C11" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>9</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>9</v>
@@ -7616,12 +8181,12 @@
       <c r="M11" s="7"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="B12" s="87"/>
-      <c r="C12" s="103" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>5</v>
+      <c r="B12" s="91"/>
+      <c r="C12" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>9</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>9</v>
@@ -7650,12 +8215,12 @@
       <c r="M12" s="7"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="B13" s="87"/>
-      <c r="C13" s="105" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>5</v>
+      <c r="B13" s="91"/>
+      <c r="C13" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>9</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>9</v>
@@ -7690,16 +8255,16 @@
       <c r="C17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="99" t="s">
+      <c r="D17" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="100"/>
-      <c r="F17" s="100"/>
-      <c r="G17" s="100"/>
-      <c r="H17" s="100"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="52"/>
-      <c r="K17" s="52"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="90"/>
+      <c r="H17" s="90"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="50"/>
     </row>
     <row r="18" spans="2:11" ht="20.25" customHeight="1">
       <c r="B18" s="15">
@@ -7708,16 +8273,16 @@
       <c r="C18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="98" t="s">
+      <c r="D18" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="98"/>
-      <c r="F18" s="98"/>
-      <c r="G18" s="98"/>
-      <c r="H18" s="98"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="53"/>
+      <c r="E18" s="88"/>
+      <c r="F18" s="88"/>
+      <c r="G18" s="88"/>
+      <c r="H18" s="88"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
     </row>
     <row r="19" spans="2:11" s="6" customFormat="1">
       <c r="B19" s="8">
@@ -7726,16 +8291,16 @@
       <c r="C19" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="98" t="s">
+      <c r="D19" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="98"/>
-      <c r="F19" s="98"/>
-      <c r="G19" s="98"/>
-      <c r="H19" s="98"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="53"/>
+      <c r="E19" s="88"/>
+      <c r="F19" s="88"/>
+      <c r="G19" s="88"/>
+      <c r="H19" s="88"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
     </row>
     <row r="20" spans="2:11">
       <c r="B20" s="15">
@@ -7744,16 +8309,16 @@
       <c r="C20" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="98" t="s">
+      <c r="D20" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="98"/>
-      <c r="F20" s="98"/>
-      <c r="G20" s="98"/>
-      <c r="H20" s="98"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
-      <c r="K20" s="53"/>
+      <c r="E20" s="88"/>
+      <c r="F20" s="88"/>
+      <c r="G20" s="88"/>
+      <c r="H20" s="88"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
     </row>
     <row r="21" spans="2:11" ht="47.25" customHeight="1">
       <c r="B21" s="15">
@@ -7762,16 +8327,16 @@
       <c r="C21" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="98" t="s">
+      <c r="D21" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="98"/>
-      <c r="F21" s="98"/>
-      <c r="G21" s="98"/>
-      <c r="H21" s="98"/>
-      <c r="I21" s="53"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="53"/>
+      <c r="E21" s="88"/>
+      <c r="F21" s="88"/>
+      <c r="G21" s="88"/>
+      <c r="H21" s="88"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
     </row>
     <row r="22" spans="2:11" ht="49.5" customHeight="1">
       <c r="B22" s="15">
@@ -7780,16 +8345,16 @@
       <c r="C22" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="98" t="s">
+      <c r="D22" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="98"/>
-      <c r="F22" s="98"/>
-      <c r="G22" s="98"/>
-      <c r="H22" s="98"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="53"/>
+      <c r="E22" s="88"/>
+      <c r="F22" s="88"/>
+      <c r="G22" s="88"/>
+      <c r="H22" s="88"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="51"/>
     </row>
     <row r="23" spans="2:11" ht="78.75" customHeight="1">
       <c r="B23" s="15">
@@ -7798,19 +8363,26 @@
       <c r="C23" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="98" t="s">
+      <c r="D23" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="98"/>
-      <c r="F23" s="98"/>
-      <c r="G23" s="98"/>
-      <c r="H23" s="98"/>
-      <c r="I23" s="53"/>
-      <c r="J23" s="53"/>
-      <c r="K23" s="53"/>
+      <c r="E23" s="88"/>
+      <c r="F23" s="88"/>
+      <c r="G23" s="88"/>
+      <c r="H23" s="88"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:K2"/>
     <mergeCell ref="D21:H21"/>
     <mergeCell ref="D23:H23"/>
     <mergeCell ref="D22:H22"/>
@@ -7818,25 +8390,18 @@
     <mergeCell ref="D17:H17"/>
     <mergeCell ref="D20:H20"/>
     <mergeCell ref="D18:H18"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B1:L1"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:K2"/>
   </mergeCells>
-  <conditionalFormatting sqref="C19 G10 D5:D13 F8:F9 G8:H8 J9:J13 I7:I13 J7 K6:K13 I4:K4 M4:M13 L4:L6 L10:L13">
-    <cfRule type="containsText" dxfId="27" priority="1873" operator="containsText" text="Not Aware">
+  <conditionalFormatting sqref="C19 G10 L10:L13 F8:F9 J9:J13 I7:I13 I4:K4 M4:M13 L4:L6 G8:H8 J7 K6:K13">
+    <cfRule type="containsText" dxfId="51" priority="1873" operator="containsText" text="Not Aware">
       <formula>NOT(ISERROR(SEARCH("Not Aware",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="1874" operator="containsText" text="Beginner">
+    <cfRule type="containsText" dxfId="50" priority="1874" operator="containsText" text="Beginner">
       <formula>NOT(ISERROR(SEARCH("Beginner",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="1875" operator="containsText" text="Intermediate">
+    <cfRule type="containsText" dxfId="49" priority="1875" operator="containsText" text="Intermediate">
       <formula>NOT(ISERROR(SEARCH("Intermediate",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="1876" operator="containsText" text="Expert">
+    <cfRule type="containsText" dxfId="48" priority="1876" operator="containsText" text="Expert">
       <formula>NOT(ISERROR(SEARCH("Expert",C4)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7849,8 +8414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:M23"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:H8"/>
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7872,69 +8437,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="18.75">
-      <c r="B1" s="88" t="s">
+      <c r="B1" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
       <c r="M1" s="24"/>
     </row>
     <row r="2" spans="2:13">
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="93" t="s">
+      <c r="C2" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="95" t="s">
+      <c r="D2" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="91" t="s">
+      <c r="E2" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="91" t="s">
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="103"/>
     </row>
     <row r="3" spans="2:13" ht="31.5" customHeight="1">
-      <c r="B3" s="94"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="96"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="98"/>
       <c r="E3" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="H3" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="I3" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="J3" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="K3" s="24" t="s">
         <v>66</v>
-      </c>
-      <c r="J3" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="K3" s="24" t="s">
-        <v>68</v>
       </c>
       <c r="L3" s="24" t="s">
         <v>58</v>
@@ -7944,7 +8509,7 @@
       </c>
     </row>
     <row r="4" spans="2:13" ht="30" customHeight="1">
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="49" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -7984,22 +8549,22 @@
         <v>29</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>6</v>
+      <c r="E5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="I5" s="14" t="s">
         <v>9</v>
@@ -8018,25 +8583,25 @@
     <row r="6" spans="2:13" ht="15.75">
       <c r="B6" s="102"/>
       <c r="C6" s="28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>6</v>
+      <c r="E6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>4</v>
@@ -8052,7 +8617,7 @@
     <row r="7" spans="2:13" ht="15.75">
       <c r="B7" s="102"/>
       <c r="C7" s="28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>5</v>
@@ -8086,7 +8651,7 @@
     <row r="8" spans="2:13" ht="15.75">
       <c r="B8" s="102"/>
       <c r="C8" s="28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>5</v>
@@ -8120,7 +8685,7 @@
     <row r="9" spans="2:13">
       <c r="B9" s="102"/>
       <c r="C9" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>5</v>
@@ -8152,20 +8717,20 @@
       <c r="M9" s="7"/>
     </row>
     <row r="10" spans="2:13" ht="15.75">
-      <c r="B10" s="87" t="s">
+      <c r="B10" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="54" t="s">
-        <v>84</v>
+      <c r="C10" s="52" t="s">
+        <v>82</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>6</v>
+      <c r="E10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>6</v>
@@ -8188,7 +8753,7 @@
       <c r="M10" s="7"/>
     </row>
     <row r="11" spans="2:13">
-      <c r="B11" s="87"/>
+      <c r="B11" s="91"/>
       <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
@@ -8222,9 +8787,9 @@
       <c r="M11" s="7"/>
     </row>
     <row r="12" spans="2:13">
-      <c r="B12" s="87"/>
+      <c r="B12" s="91"/>
       <c r="C12" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>5</v>
@@ -8256,7 +8821,7 @@
       <c r="M12" s="7"/>
     </row>
     <row r="13" spans="2:13">
-      <c r="B13" s="87"/>
+      <c r="B13" s="91"/>
       <c r="C13" s="29" t="s">
         <v>31</v>
       </c>
@@ -8296,13 +8861,13 @@
       <c r="C17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="99" t="s">
+      <c r="D17" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="100"/>
-      <c r="F17" s="100"/>
-      <c r="G17" s="100"/>
-      <c r="H17" s="100"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="90"/>
+      <c r="H17" s="90"/>
     </row>
     <row r="18" spans="2:8" ht="20.25" customHeight="1">
       <c r="B18" s="15">
@@ -8311,13 +8876,13 @@
       <c r="C18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="98" t="s">
+      <c r="D18" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="98"/>
-      <c r="F18" s="98"/>
-      <c r="G18" s="98"/>
-      <c r="H18" s="98"/>
+      <c r="E18" s="88"/>
+      <c r="F18" s="88"/>
+      <c r="G18" s="88"/>
+      <c r="H18" s="88"/>
     </row>
     <row r="19" spans="2:8">
       <c r="B19" s="8">
@@ -8326,13 +8891,13 @@
       <c r="C19" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="98" t="s">
+      <c r="D19" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="98"/>
-      <c r="F19" s="98"/>
-      <c r="G19" s="98"/>
-      <c r="H19" s="98"/>
+      <c r="E19" s="88"/>
+      <c r="F19" s="88"/>
+      <c r="G19" s="88"/>
+      <c r="H19" s="88"/>
     </row>
     <row r="20" spans="2:8">
       <c r="B20" s="15">
@@ -8341,13 +8906,13 @@
       <c r="C20" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="98" t="s">
+      <c r="D20" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="98"/>
-      <c r="F20" s="98"/>
-      <c r="G20" s="98"/>
-      <c r="H20" s="98"/>
+      <c r="E20" s="88"/>
+      <c r="F20" s="88"/>
+      <c r="G20" s="88"/>
+      <c r="H20" s="88"/>
     </row>
     <row r="21" spans="2:8" ht="47.25" customHeight="1">
       <c r="B21" s="15">
@@ -8356,13 +8921,13 @@
       <c r="C21" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="98" t="s">
+      <c r="D21" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="98"/>
-      <c r="F21" s="98"/>
-      <c r="G21" s="98"/>
-      <c r="H21" s="98"/>
+      <c r="E21" s="88"/>
+      <c r="F21" s="88"/>
+      <c r="G21" s="88"/>
+      <c r="H21" s="88"/>
     </row>
     <row r="22" spans="2:8" ht="49.5" customHeight="1">
       <c r="B22" s="15">
@@ -8371,13 +8936,13 @@
       <c r="C22" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="98" t="s">
+      <c r="D22" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="98"/>
-      <c r="F22" s="98"/>
-      <c r="G22" s="98"/>
-      <c r="H22" s="98"/>
+      <c r="E22" s="88"/>
+      <c r="F22" s="88"/>
+      <c r="G22" s="88"/>
+      <c r="H22" s="88"/>
     </row>
     <row r="23" spans="2:8" ht="78.75" customHeight="1">
       <c r="B23" s="15">
@@ -8386,16 +8951,22 @@
       <c r="C23" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="98" t="s">
+      <c r="D23" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="98"/>
-      <c r="F23" s="98"/>
-      <c r="G23" s="98"/>
-      <c r="H23" s="98"/>
+      <c r="E23" s="88"/>
+      <c r="F23" s="88"/>
+      <c r="G23" s="88"/>
+      <c r="H23" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="D22:H22"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="D17:H17"/>
+    <mergeCell ref="D18:H18"/>
+    <mergeCell ref="D19:H19"/>
+    <mergeCell ref="D20:H20"/>
     <mergeCell ref="B5:B9"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="D21:H21"/>
@@ -8405,39 +8976,89 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
-    <mergeCell ref="D22:H22"/>
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="D17:H17"/>
-    <mergeCell ref="D18:H18"/>
-    <mergeCell ref="D19:H19"/>
-    <mergeCell ref="D20:H20"/>
   </mergeCells>
   <conditionalFormatting sqref="M5:M13 J5:J9 K5:L8 L9:L13 J5:L7 C19 E9 H4:M4 J10:L13 D5:D13 E11:I13 I7:I9 G9:L9">
-    <cfRule type="containsText" dxfId="19" priority="453" operator="containsText" text="Not Aware">
+    <cfRule type="containsText" dxfId="83" priority="469" operator="containsText" text="Not Aware">
       <formula>NOT(ISERROR(SEARCH("Not Aware",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="454" operator="containsText" text="Beginner">
+    <cfRule type="containsText" dxfId="82" priority="470" operator="containsText" text="Beginner">
       <formula>NOT(ISERROR(SEARCH("Beginner",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="455" operator="containsText" text="Intermediate">
+    <cfRule type="containsText" dxfId="81" priority="471" operator="containsText" text="Intermediate">
       <formula>NOT(ISERROR(SEARCH("Intermediate",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="456" operator="containsText" text="Expert">
+    <cfRule type="containsText" dxfId="80" priority="472" operator="containsText" text="Expert">
       <formula>NOT(ISERROR(SEARCH("Expert",C4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J30:L30">
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Not Aware">
+    <cfRule type="containsText" dxfId="79" priority="17" operator="containsText" text="Not Aware">
       <formula>NOT(ISERROR(SEARCH("Not Aware",J30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="Beginner">
+    <cfRule type="containsText" dxfId="78" priority="18" operator="containsText" text="Beginner">
       <formula>NOT(ISERROR(SEARCH("Beginner",J30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Intermediate">
+    <cfRule type="containsText" dxfId="77" priority="19" operator="containsText" text="Intermediate">
       <formula>NOT(ISERROR(SEARCH("Intermediate",J30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Expert">
+    <cfRule type="containsText" dxfId="76" priority="20" operator="containsText" text="Expert">
       <formula>NOT(ISERROR(SEARCH("Expert",J30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:H5">
+    <cfRule type="containsText" dxfId="31" priority="13" operator="containsText" text="Not Aware">
+      <formula>NOT(ISERROR(SEARCH("Not Aware",E5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="14" operator="containsText" text="Beginner">
+      <formula>NOT(ISERROR(SEARCH("Beginner",E5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="15" operator="containsText" text="Intermediate">
+      <formula>NOT(ISERROR(SEARCH("Intermediate",E5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="16" operator="containsText" text="Expert">
+      <formula>NOT(ISERROR(SEARCH("Expert",E5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6:H6">
+    <cfRule type="containsText" dxfId="23" priority="9" operator="containsText" text="Not Aware">
+      <formula>NOT(ISERROR(SEARCH("Not Aware",E6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="10" operator="containsText" text="Beginner">
+      <formula>NOT(ISERROR(SEARCH("Beginner",E6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="11" operator="containsText" text="Intermediate">
+      <formula>NOT(ISERROR(SEARCH("Intermediate",E6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="12" operator="containsText" text="Expert">
+      <formula>NOT(ISERROR(SEARCH("Expert",E6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6">
+    <cfRule type="containsText" dxfId="15" priority="5" operator="containsText" text="Not Aware">
+      <formula>NOT(ISERROR(SEARCH("Not Aware",I6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="6" operator="containsText" text="Beginner">
+      <formula>NOT(ISERROR(SEARCH("Beginner",I6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="Intermediate">
+      <formula>NOT(ISERROR(SEARCH("Intermediate",I6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="8" operator="containsText" text="Expert">
+      <formula>NOT(ISERROR(SEARCH("Expert",I6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10:F10">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Not Aware">
+      <formula>NOT(ISERROR(SEARCH("Not Aware",E10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Beginner">
+      <formula>NOT(ISERROR(SEARCH("Beginner",E10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Intermediate">
+      <formula>NOT(ISERROR(SEARCH("Intermediate",E10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Expert">
+      <formula>NOT(ISERROR(SEARCH("Expert",E10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8450,7 +9071,7 @@
   <dimension ref="A2:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A8" sqref="A8:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8497,7 +9118,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="6" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="B3" s="22">
         <f>COUNTIF('Functional Knowledge Matrix'!$E$4:$L$13,'Functional Analysis'!B$2)/$I$3</f>
@@ -8505,11 +9126,11 @@
       </c>
       <c r="C3" s="22">
         <f>COUNTIF('Functional Knowledge Matrix'!$E$4:$L$13,'Functional Analysis'!C$2)/$I$3</f>
-        <v>7.4999999999999997E-2</v>
+        <v>3.7499999999999999E-2</v>
       </c>
       <c r="D3" s="22">
         <f>COUNTIF('Functional Knowledge Matrix'!$E$4:$L$13,'Functional Analysis'!D$2)/$I$3</f>
-        <v>0.4</v>
+        <v>0.4375</v>
       </c>
       <c r="E3" s="22">
         <f>COUNTIF('Functional Knowledge Matrix'!$E$4:$L$13,'Functional Analysis'!E$2)/$I$3</f>
@@ -8554,36 +9175,43 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="6" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="B8" s="22">
-        <f>COUNTIF('Functional Knowledge Matrix'!$E$4:$L$13,'Functional Analysis'!B$2)/$I$3</f>
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="C8" s="22">
-        <f>COUNTIF('Functional Knowledge Matrix'!$E$4:$L$13,'Functional Analysis'!C$2)/$I$3</f>
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="D8" s="22">
-        <f>COUNTIF('Functional Knowledge Matrix'!$E$4:$L$13,'Functional Analysis'!D$2)/$I$3</f>
         <v>0.4</v>
       </c>
       <c r="E8" s="22">
-        <f>COUNTIF('Functional Knowledge Matrix'!$E$4:$L$13,'Functional Analysis'!E$2)/$I$3</f>
         <v>0</v>
       </c>
       <c r="F8" s="22">
-        <f>COUNTIF('Functional Knowledge Matrix'!$E$4:$L$13,'Functional Analysis'!F$2)/$I$3</f>
         <v>0.51249999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="1"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
+      <c r="A9" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="18">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="C9" s="18">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="D9" s="18">
+        <v>0.4375</v>
+      </c>
+      <c r="E9" s="18">
+        <v>0</v>
+      </c>
+      <c r="F9" s="18">
+        <v>0.51249999999999996</v>
+      </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1"/>
@@ -8604,7 +9232,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B9" sqref="B9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8654,7 +9282,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="6" t="s">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="B3" s="22">
         <f>COUNTIF('Technical Knowledge Matrix'!$E$4:$L$10,'Technical Analysis'!B$2)/$I$3</f>
@@ -8662,11 +9290,11 @@
       </c>
       <c r="C3" s="22">
         <f>COUNTIF('Technical Knowledge Matrix'!$E$4:$L$10,'Technical Analysis'!C$2)/$I$3</f>
-        <v>0.3783783783783784</v>
+        <v>8.1081081081081086E-2</v>
       </c>
       <c r="D3" s="22">
         <f>COUNTIF('Technical Knowledge Matrix'!$E$4:$L$10,'Technical Analysis'!D$2)/$I$3</f>
-        <v>0.24324324324324326</v>
+        <v>0.54054054054054057</v>
       </c>
       <c r="E3" s="22">
         <f>COUNTIF('Technical Knowledge Matrix'!$E$4:$L$10,'Technical Analysis'!E$2)/$I$3</f>
@@ -8711,36 +9339,43 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="6" t="s">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="B8" s="22">
-        <f>COUNTIF('Technical Knowledge Matrix'!$E$4:$L$10,'Technical Analysis'!B$2)/$I$3</f>
         <v>0</v>
       </c>
       <c r="C8" s="22">
-        <f>COUNTIF('Technical Knowledge Matrix'!$E$4:$L$10,'Technical Analysis'!C$2)/$I$3</f>
         <v>0.3783783783783784</v>
       </c>
       <c r="D8" s="22">
-        <f>COUNTIF('Technical Knowledge Matrix'!$E$4:$L$10,'Technical Analysis'!D$2)/$I$3</f>
         <v>0.24324324324324326</v>
       </c>
       <c r="E8" s="22">
-        <f>COUNTIF('Technical Knowledge Matrix'!$E$4:$L$10,'Technical Analysis'!E$2)/$I$3</f>
         <v>0</v>
       </c>
       <c r="F8" s="22">
-        <f>COUNTIF('Technical Knowledge Matrix'!$E$4:$L$10,'Technical Analysis'!F$2)/$I$3</f>
         <v>0.3783783783783784</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="1"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
+      <c r="A9" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="18">
+        <v>0</v>
+      </c>
+      <c r="C9" s="18">
+        <v>8.1081081081081086E-2</v>
+      </c>
+      <c r="D9" s="18">
+        <v>0.54054054054054057</v>
+      </c>
+      <c r="E9" s="18">
+        <v>0</v>
+      </c>
+      <c r="F9" s="18">
+        <v>0.3783783783783784</v>
+      </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1"/>
@@ -8761,266 +9396,294 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="6" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="18.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="2" customWidth="1"/>
+    <col min="5" max="7" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="104" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="104" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="104" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="104" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="104" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="104" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+    <row r="2" spans="1:7" ht="60">
+      <c r="A2" s="105" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="105"/>
+      <c r="C2" s="105" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="105" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="105" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="60">
+      <c r="A3" s="105" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="105"/>
+      <c r="C3" s="105" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="105" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="105" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="75">
+      <c r="A4" s="105" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="105"/>
+      <c r="C4" s="105" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="105" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="105" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="105"/>
+      <c r="G4" s="105" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="A5" s="105"/>
+      <c r="B5" s="105"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="105"/>
+      <c r="G5" s="105"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="A6" s="105"/>
+      <c r="B6" s="105"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="105"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="A7" s="105"/>
+      <c r="B7" s="105"/>
+      <c r="C7" s="105"/>
+      <c r="D7" s="105"/>
+      <c r="E7" s="105"/>
+      <c r="F7" s="105"/>
+      <c r="G7" s="105"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="A8" s="105"/>
+      <c r="B8" s="105"/>
+      <c r="C8" s="105"/>
+      <c r="D8" s="105"/>
+      <c r="E8" s="105"/>
+      <c r="F8" s="105"/>
+      <c r="G8" s="105"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="A9" s="105"/>
+      <c r="B9" s="105"/>
+      <c r="C9" s="105"/>
+      <c r="D9" s="105"/>
+      <c r="E9" s="105"/>
+      <c r="F9" s="105"/>
+      <c r="G9" s="105"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="A10" s="105"/>
+      <c r="B10" s="105"/>
+      <c r="C10" s="105"/>
+      <c r="D10" s="105"/>
+      <c r="E10" s="105"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="105"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="A11" s="105"/>
+      <c r="B11" s="105"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="105"/>
+      <c r="E11" s="105"/>
+      <c r="F11" s="105"/>
+      <c r="G11" s="105"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="A12" s="105"/>
+      <c r="B12" s="105"/>
+      <c r="C12" s="105"/>
+      <c r="D12" s="105"/>
+      <c r="E12" s="105"/>
+      <c r="F12" s="105"/>
+      <c r="G12" s="105"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="A13" s="105"/>
+      <c r="B13" s="105"/>
+      <c r="C13" s="105"/>
+      <c r="D13" s="105"/>
+      <c r="E13" s="105"/>
+      <c r="F13" s="105"/>
+      <c r="G13" s="105"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="A14" s="105"/>
+      <c r="B14" s="105"/>
+      <c r="C14" s="105"/>
+      <c r="D14" s="105"/>
+      <c r="E14" s="105"/>
+      <c r="F14" s="105"/>
+      <c r="G14" s="105"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="A15" s="105"/>
+      <c r="B15" s="105"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="105"/>
+      <c r="G15" s="105"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="A16" s="105"/>
+      <c r="B16" s="105"/>
+      <c r="C16" s="105"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="105"/>
+      <c r="F16" s="105"/>
+      <c r="G16" s="105"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="A17" s="105"/>
+      <c r="B17" s="105"/>
+      <c r="C17" s="105"/>
+      <c r="D17" s="105"/>
+      <c r="E17" s="105"/>
+      <c r="F17" s="105"/>
+      <c r="G17" s="105"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="A18" s="105"/>
+      <c r="B18" s="105"/>
+      <c r="C18" s="105"/>
+      <c r="D18" s="105"/>
+      <c r="E18" s="105"/>
+      <c r="F18" s="105"/>
+      <c r="G18" s="105"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="A19" s="105"/>
+      <c r="B19" s="105"/>
+      <c r="C19" s="105"/>
+      <c r="D19" s="105"/>
+      <c r="E19" s="105"/>
+      <c r="F19" s="105"/>
+      <c r="G19" s="105"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="A20" s="105"/>
+      <c r="B20" s="105"/>
+      <c r="C20" s="105"/>
+      <c r="D20" s="105"/>
+      <c r="E20" s="105"/>
+      <c r="F20" s="105"/>
+      <c r="G20" s="105"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="A21" s="105"/>
+      <c r="B21" s="105"/>
+      <c r="C21" s="105"/>
+      <c r="D21" s="105"/>
+      <c r="E21" s="105"/>
+      <c r="F21" s="105"/>
+      <c r="G21" s="105"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="A22" s="105"/>
+      <c r="B22" s="105"/>
+      <c r="C22" s="105"/>
+      <c r="D22" s="105"/>
+      <c r="E22" s="105"/>
+      <c r="F22" s="105"/>
+      <c r="G22" s="105"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="A23" s="105"/>
+      <c r="B23" s="105"/>
+      <c r="C23" s="105"/>
+      <c r="D23" s="105"/>
+      <c r="E23" s="105"/>
+      <c r="F23" s="105"/>
+      <c r="G23" s="105"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="A24" s="105"/>
+      <c r="B24" s="105"/>
+      <c r="C24" s="105"/>
+      <c r="D24" s="105"/>
+      <c r="E24" s="105"/>
+      <c r="F24" s="105"/>
+      <c r="G24" s="105"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+      <c r="A25" s="105"/>
+      <c r="B25" s="105"/>
+      <c r="C25" s="105"/>
+      <c r="D25" s="105"/>
+      <c r="E25" s="105"/>
+      <c r="F25" s="105"/>
+      <c r="G25" s="105"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="A26" s="105"/>
+      <c r="B26" s="105"/>
+      <c r="C26" s="105"/>
+      <c r="D26" s="105"/>
+      <c r="E26" s="105"/>
+      <c r="F26" s="105"/>
+      <c r="G26" s="105"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>